<commit_message>
There'a a loop in InitPWM .
</commit_message>
<xml_diff>
--- a/Scheme.xlsx
+++ b/Scheme.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>SN76496</t>
   </si>
@@ -87,9 +87,6 @@
     <t>PC3</t>
   </si>
   <si>
-    <t>PA8</t>
-  </si>
-  <si>
     <t>PC4</t>
   </si>
   <si>
@@ -108,10 +105,10 @@
     <t>PC9</t>
   </si>
   <si>
-    <t>PC10</t>
-  </si>
-  <si>
     <t>Audio Jack</t>
+  </si>
+  <si>
+    <t>PA6</t>
   </si>
 </sst>
 </file>
@@ -327,66 +324,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -669,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H1:W31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,29 +685,29 @@
   <sheetData>
     <row r="1" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="6"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="16"/>
     </row>
     <row r="3" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="3" t="s">
+      <c r="I3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="7" t="s">
+      <c r="K3" s="17"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="P3" t="s">
@@ -718,29 +715,29 @@
       </c>
     </row>
     <row r="4" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J4" s="8"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="8"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="4"/>
     </row>
     <row r="5" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H5" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="3" t="s">
+      <c r="I5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="9"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="7" t="s">
+      <c r="K5" s="17"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="P5" t="s">
@@ -748,287 +745,290 @@
       </c>
     </row>
     <row r="6" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J6" s="8"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="8"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="4"/>
     </row>
     <row r="7" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H7" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="3" t="s">
+      <c r="I7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="7" t="s">
+      <c r="K7" s="17"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="15" t="s">
+      <c r="O7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="P7" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J8" s="8"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="8"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="4"/>
     </row>
     <row r="9" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="9"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="7" t="s">
+      <c r="K9" s="17"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O9" s="15" t="s">
+      <c r="O9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="P9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J10" s="8"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="8"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="4"/>
     </row>
     <row r="11" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="7" t="s">
+      <c r="K11" s="17"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O11" s="15" t="s">
+      <c r="O11" s="5" t="s">
         <v>17</v>
       </c>
       <c r="P11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J12" s="8"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="8"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="4"/>
     </row>
     <row r="13" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H13" t="s">
-        <v>29</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="9"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="7" t="s">
+      <c r="K13" s="17"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O13" s="15" t="s">
+      <c r="O13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="P13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J14" s="4"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" s="17"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J14" s="8"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="8"/>
-    </row>
-    <row r="15" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I15" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K15" s="9"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="O15" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="P15" t="s">
-        <v>26</v>
-      </c>
-    </row>
     <row r="16" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J16" s="8"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="8"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="4"/>
     </row>
     <row r="17" spans="8:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H17" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="J17" s="3" t="s">
+      <c r="I17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K17" s="9"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="7" t="s">
+      <c r="K17" s="17"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="O17" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="S17" s="19" t="s">
+      <c r="O17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P17" t="s">
+        <v>8</v>
+      </c>
+      <c r="S17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T17" s="22"/>
-      <c r="U17" s="22"/>
-      <c r="V17" s="22"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
     </row>
     <row r="18" spans="8:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J18" s="8"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="8"/>
-      <c r="T18" s="22"/>
-      <c r="U18" s="22"/>
-      <c r="V18" s="22"/>
-      <c r="W18" s="21"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="4"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="7"/>
     </row>
     <row r="19" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="R19" s="15"/>
-      <c r="S19" s="19" t="s">
+      <c r="R19" s="5"/>
+      <c r="S19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="T19" s="22"/>
-      <c r="U19" s="22"/>
-      <c r="V19" s="22"/>
-      <c r="W19" s="16"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="9"/>
     </row>
     <row r="20" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="T20" s="22"/>
-      <c r="U20" s="23" t="s">
+      <c r="T20" s="13"/>
+      <c r="U20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="V20" s="22"/>
-      <c r="W20" s="17"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="10"/>
     </row>
     <row r="21" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="R21" s="15"/>
-      <c r="S21" s="19" t="s">
+      <c r="R21" s="5"/>
+      <c r="S21" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="T21" s="22"/>
-      <c r="U21" s="22"/>
-      <c r="V21" s="22"/>
-      <c r="W21" s="18"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="13"/>
+      <c r="W21" s="11"/>
     </row>
     <row r="22" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="T22" s="22"/>
-      <c r="U22" s="22"/>
-      <c r="V22" s="22"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="13"/>
     </row>
     <row r="23" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="S23" s="19" t="s">
+      <c r="S23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T23" s="22"/>
-      <c r="U23" s="22"/>
-      <c r="V23" s="22"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13"/>
     </row>
     <row r="24" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="T24" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="U24" s="20"/>
-      <c r="V24" s="20"/>
+      <c r="T24" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="U24" s="12"/>
+      <c r="V24" s="12"/>
     </row>
     <row r="26" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
       <c r="M26" s="1"/>
     </row>
     <row r="27" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
     </row>
     <row r="28" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="I28" s="2"/>
-      <c r="K28" s="2"/>
+      <c r="I28" s="23"/>
+      <c r="K28" s="23"/>
     </row>
     <row r="29" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
     </row>
     <row r="30" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
     </row>
     <row r="31" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="K2:M18"/>
+    <mergeCell ref="I26:I31"/>
+    <mergeCell ref="K26:K31"/>
+    <mergeCell ref="J29:J31"/>
+    <mergeCell ref="J26:J27"/>
     <mergeCell ref="W19:W21"/>
     <mergeCell ref="T24:V24"/>
     <mergeCell ref="T17:T23"/>
     <mergeCell ref="V17:V23"/>
     <mergeCell ref="U21:U23"/>
     <mergeCell ref="U17:U19"/>
-    <mergeCell ref="K2:M18"/>
-    <mergeCell ref="I26:I31"/>
-    <mergeCell ref="K26:K31"/>
-    <mergeCell ref="J29:J31"/>
-    <mergeCell ref="J26:J27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
trying to build an SN76496 LIB
</commit_message>
<xml_diff>
--- a/Scheme.xlsx
+++ b/Scheme.xlsx
@@ -339,6 +339,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -352,36 +382,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -685,11 +685,11 @@
   <sheetData>
     <row r="1" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="15"/>
-      <c r="M2" s="16"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="11"/>
     </row>
     <row r="3" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H3" t="s">
@@ -701,9 +701,9 @@
       <c r="J3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="17"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="19"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="14"/>
       <c r="N3" s="3" t="s">
         <v>9</v>
       </c>
@@ -716,9 +716,9 @@
     </row>
     <row r="4" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J4" s="4"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="19"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="14"/>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -731,9 +731,9 @@
       <c r="J5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="19"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="14"/>
       <c r="N5" s="3" t="s">
         <v>10</v>
       </c>
@@ -746,9 +746,9 @@
     </row>
     <row r="6" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J6" s="4"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="19"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="14"/>
       <c r="N6" s="4"/>
     </row>
     <row r="7" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -761,9 +761,9 @@
       <c r="J7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="17"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="19"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="14"/>
       <c r="N7" s="3" t="s">
         <v>11</v>
       </c>
@@ -776,9 +776,9 @@
     </row>
     <row r="8" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J8" s="4"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="19"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="14"/>
       <c r="N8" s="4"/>
     </row>
     <row r="9" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -791,9 +791,9 @@
       <c r="J9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="17"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="19"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="14"/>
       <c r="N9" s="3" t="s">
         <v>12</v>
       </c>
@@ -806,9 +806,9 @@
     </row>
     <row r="10" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J10" s="4"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="19"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="14"/>
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -821,9 +821,9 @@
       <c r="J11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K11" s="17"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="19"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="14"/>
       <c r="N11" s="3" t="s">
         <v>13</v>
       </c>
@@ -836,9 +836,9 @@
     </row>
     <row r="12" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J12" s="4"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="19"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="14"/>
       <c r="N12" s="4"/>
     </row>
     <row r="13" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -851,9 +851,9 @@
       <c r="J13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="17"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="19"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="14"/>
       <c r="N13" s="3" t="s">
         <v>14</v>
       </c>
@@ -866,9 +866,9 @@
     </row>
     <row r="14" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J14" s="4"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="19"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="14"/>
       <c r="N14" s="4"/>
     </row>
     <row r="15" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -878,9 +878,9 @@
       <c r="J15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K15" s="17"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="19"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="14"/>
       <c r="N15" s="3" t="s">
         <v>15</v>
       </c>
@@ -893,9 +893,9 @@
     </row>
     <row r="16" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J16" s="4"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="19"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="14"/>
       <c r="N16" s="4"/>
     </row>
     <row r="17" spans="8:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -908,9 +908,9 @@
       <c r="J17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K17" s="17"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="19"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="14"/>
       <c r="N17" s="3" t="s">
         <v>16</v>
       </c>
@@ -923,19 +923,19 @@
       <c r="S17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="13"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
     </row>
     <row r="18" spans="8:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J18" s="4"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="22"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="17"/>
       <c r="N18" s="4"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
+      <c r="T18" s="23"/>
+      <c r="U18" s="23"/>
+      <c r="V18" s="23"/>
       <c r="W18" s="7"/>
     </row>
     <row r="19" spans="8:23" x14ac:dyDescent="0.25">
@@ -943,92 +943,92 @@
       <c r="S19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
-      <c r="V19" s="13"/>
-      <c r="W19" s="9"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
+      <c r="W19" s="19"/>
     </row>
     <row r="20" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="T20" s="13"/>
+      <c r="T20" s="23"/>
       <c r="U20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="V20" s="13"/>
-      <c r="W20" s="10"/>
+      <c r="V20" s="23"/>
+      <c r="W20" s="20"/>
     </row>
     <row r="21" spans="8:23" x14ac:dyDescent="0.25">
       <c r="R21" s="5"/>
       <c r="S21" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="13"/>
-      <c r="W21" s="11"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="21"/>
     </row>
     <row r="22" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="T22" s="13"/>
-      <c r="U22" s="13"/>
-      <c r="V22" s="13"/>
+      <c r="T22" s="23"/>
+      <c r="U22" s="23"/>
+      <c r="V22" s="23"/>
     </row>
     <row r="23" spans="8:23" x14ac:dyDescent="0.25">
       <c r="S23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T23" s="13"/>
-      <c r="U23" s="13"/>
-      <c r="V23" s="13"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+      <c r="V23" s="23"/>
     </row>
     <row r="24" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="T24" s="12" t="s">
+      <c r="T24" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="U24" s="12"/>
-      <c r="V24" s="12"/>
+      <c r="U24" s="22"/>
+      <c r="V24" s="22"/>
     </row>
     <row r="26" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
       <c r="M26" s="1"/>
     </row>
     <row r="27" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
     </row>
     <row r="28" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="I28" s="23"/>
-      <c r="K28" s="23"/>
+      <c r="I28" s="18"/>
+      <c r="K28" s="18"/>
     </row>
     <row r="29" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
     </row>
     <row r="30" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
     </row>
     <row r="31" spans="8:23" x14ac:dyDescent="0.25">
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="K2:M18"/>
-    <mergeCell ref="I26:I31"/>
-    <mergeCell ref="K26:K31"/>
-    <mergeCell ref="J29:J31"/>
-    <mergeCell ref="J26:J27"/>
     <mergeCell ref="W19:W21"/>
     <mergeCell ref="T24:V24"/>
     <mergeCell ref="T17:T23"/>
     <mergeCell ref="V17:V23"/>
     <mergeCell ref="U21:U23"/>
     <mergeCell ref="U17:U19"/>
+    <mergeCell ref="K2:M18"/>
+    <mergeCell ref="I26:I31"/>
+    <mergeCell ref="K26:K31"/>
+    <mergeCell ref="J29:J31"/>
+    <mergeCell ref="J26:J27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>